<commit_message>
Dictionary Engine - null filter fix
</commit_message>
<xml_diff>
--- a/SchVictorina.WebAPI/Config/rivers.xlsx
+++ b/SchVictorina.WebAPI/Config/rivers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\schvictorina\schvictorina\SchVictorina.WebAPI\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0CEA5D-4D4E-49C7-9E38-610D37C7EBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E55729-9945-46D5-AF51-26BB9F16028C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F4C5060-D6C0-4319-8B9F-A5EA184C6378}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3F4C5060-D6C0-4319-8B9F-A5EA184C6378}"/>
   </bookViews>
   <sheets>
     <sheet name="Данные" sheetId="2" r:id="rId1"/>
@@ -867,9 +867,6 @@
     <t>Какая река впадает в {Впадает в}</t>
   </si>
   <si>
-    <t>Во что впадает река {Река}?</t>
-  </si>
-  <si>
     <t>Пясина</t>
   </si>
   <si>
@@ -901,6 +898,9 @@
   </si>
   <si>
     <t>Воронеж</t>
+  </si>
+  <si>
+    <t>Во что впадает река {Название}?</t>
   </si>
 </sst>
 </file>
@@ -1355,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB528420-7780-449B-9733-531323FF703A}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>130</v>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>133</v>
@@ -1914,7 +1914,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>96</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>91</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>258</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>160</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>205</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>261</v>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>262</v>
@@ -2322,7 +2322,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>202</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>136</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>257</v>
@@ -2689,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF99941-53E7-45AA-9340-AE25C5ED6C6A}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>

</xml_diff>